<commit_message>
fixed bugs due to stale code & errors in test data
</commit_message>
<xml_diff>
--- a/testcases/test-data/functions/FloorCeilingMath.xlsx
+++ b/testcases/test-data/functions/FloorCeilingMath.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26717"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{269B9443-610C-4237-AFBE-B65CAD67B13D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F805C375-D505-4392-99B4-CC792B4F620B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="-110" windowWidth="37550" windowHeight="21820" activeTab="2" xr2:uid="{749446AB-7296-4EAA-B1ED-6089C1385F5A}"/>
+    <workbookView xWindow="8650" yWindow="1830" windowWidth="28000" windowHeight="15910" activeTab="2" xr2:uid="{749446AB-7296-4EAA-B1ED-6089C1385F5A}"/>
   </bookViews>
   <sheets>
     <sheet name="CEILING,FALSE" sheetId="1" r:id="rId1"/>
@@ -106,10 +106,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -432,7 +428,7 @@
   <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -498,7 +494,7 @@
         <v>-0.2</v>
       </c>
       <c r="S2">
-        <v>9.9999999999999603E-2</v>
+        <v>0.1</v>
       </c>
       <c r="T2">
         <v>0.4</v>
@@ -528,7 +524,7 @@
         <v>2.8</v>
       </c>
       <c r="AC2">
-        <v>3.0999999999999899</v>
+        <v>3.1</v>
       </c>
       <c r="AD2">
         <v>3.4</v>
@@ -537,13 +533,13 @@
         <v>3.7</v>
       </c>
       <c r="AF2">
-        <v>3.9999999999999898</v>
+        <v>4</v>
       </c>
       <c r="AG2">
-        <v>4.2999999999999901</v>
+        <v>4.3</v>
       </c>
       <c r="AH2">
-        <v>4.5999999999999899</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AI2">
         <v>4.9000000000000004</v>
@@ -3060,7 +3056,7 @@
       </c>
       <c r="AC20">
         <f t="shared" si="6"/>
-        <v>3.0999999999999877</v>
+        <v>3.1999999999999873</v>
       </c>
       <c r="AD20">
         <f t="shared" si="6"/>
@@ -5354,8 +5350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F87AEDF1-CBCE-4FEA-9EFE-130A4B03C9D3}">
   <dimension ref="A1:AI36"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="AH7" sqref="AH7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -5421,7 +5417,7 @@
         <v>-0.2</v>
       </c>
       <c r="S2">
-        <v>9.9999999999999603E-2</v>
+        <v>0.1</v>
       </c>
       <c r="T2">
         <v>0.4</v>
@@ -5451,7 +5447,7 @@
         <v>2.8</v>
       </c>
       <c r="AC2">
-        <v>3.0999999999999899</v>
+        <v>3.1</v>
       </c>
       <c r="AD2">
         <v>3.4</v>
@@ -5460,13 +5456,13 @@
         <v>3.7</v>
       </c>
       <c r="AF2">
-        <v>3.9999999999999898</v>
+        <v>4</v>
       </c>
       <c r="AG2">
-        <v>4.2999999999999901</v>
+        <v>4.3</v>
       </c>
       <c r="AH2">
-        <v>4.5999999999999899</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AI2">
         <v>4.9000000000000004</v>
@@ -7983,7 +7979,7 @@
       </c>
       <c r="AC20">
         <f t="shared" si="6"/>
-        <v>3.0999999999999877</v>
+        <v>3.1999999999999873</v>
       </c>
       <c r="AD20">
         <f t="shared" si="6"/>
@@ -10277,9 +10273,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7655ADE-B4DA-4A25-9412-FBC6A13AF048}">
   <dimension ref="A1:AI36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AF13" sqref="AF13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="T21" sqref="T20:T21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -10345,7 +10341,7 @@
         <v>-0.2</v>
       </c>
       <c r="S2">
-        <v>9.9999999999999603E-2</v>
+        <v>0.1</v>
       </c>
       <c r="T2">
         <v>0.4</v>
@@ -10375,7 +10371,7 @@
         <v>2.8</v>
       </c>
       <c r="AC2">
-        <v>3.0999999999999899</v>
+        <v>3.1</v>
       </c>
       <c r="AD2">
         <v>3.4</v>
@@ -10384,13 +10380,13 @@
         <v>3.7</v>
       </c>
       <c r="AF2">
-        <v>3.9999999999999898</v>
+        <v>4</v>
       </c>
       <c r="AG2">
-        <v>4.2999999999999901</v>
+        <v>4.3</v>
       </c>
       <c r="AH2">
-        <v>4.5999999999999899</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AI2">
         <v>4.9000000000000004</v>
@@ -11932,7 +11928,7 @@
       </c>
       <c r="AF13">
         <f>_xlfn.FLOOR.MATH(AF$2,$A13,$B$1)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG13">
         <f t="shared" si="2"/>
@@ -12496,7 +12492,7 @@
       </c>
       <c r="AF17">
         <f t="shared" si="2"/>
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="AG17">
         <f t="shared" si="2"/>
@@ -12637,7 +12633,7 @@
       </c>
       <c r="AF18">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="AG18">
         <f t="shared" ref="C18:AI26" si="3">_xlfn.FLOOR.MATH(AG$2,$A18,$B$1)</f>
@@ -12778,7 +12774,7 @@
       </c>
       <c r="AF19">
         <f t="shared" si="3"/>
-        <v>3.8000000000000003</v>
+        <v>4</v>
       </c>
       <c r="AG19">
         <f t="shared" si="3"/>
@@ -12786,7 +12782,7 @@
       </c>
       <c r="AH19">
         <f t="shared" si="3"/>
-        <v>4.4000000000000004</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="AI19">
         <f t="shared" si="3"/>
@@ -13060,7 +13056,7 @@
       </c>
       <c r="AF21">
         <f t="shared" si="3"/>
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="AG21">
         <f t="shared" si="3"/>
@@ -13342,7 +13338,7 @@
       </c>
       <c r="AF23">
         <f t="shared" si="3"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG23">
         <f t="shared" si="3"/>
@@ -15202,7 +15198,7 @@
   <dimension ref="A1:AI36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+      <selection activeCell="B2" sqref="B2:AI2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -15268,7 +15264,7 @@
         <v>-0.2</v>
       </c>
       <c r="S2">
-        <v>9.9999999999999603E-2</v>
+        <v>0.1</v>
       </c>
       <c r="T2">
         <v>0.4</v>
@@ -15298,7 +15294,7 @@
         <v>2.8</v>
       </c>
       <c r="AC2">
-        <v>3.0999999999999899</v>
+        <v>3.1</v>
       </c>
       <c r="AD2">
         <v>3.4</v>
@@ -15307,13 +15303,13 @@
         <v>3.7</v>
       </c>
       <c r="AF2">
-        <v>3.9999999999999898</v>
+        <v>4</v>
       </c>
       <c r="AG2">
-        <v>4.2999999999999901</v>
+        <v>4.3</v>
       </c>
       <c r="AH2">
-        <v>4.5999999999999899</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="AI2">
         <v>4.9000000000000004</v>
@@ -16855,7 +16851,7 @@
       </c>
       <c r="AF13">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AG13">
         <f t="shared" si="2"/>
@@ -17419,7 +17415,7 @@
       </c>
       <c r="AF17">
         <f t="shared" si="2"/>
-        <v>3.2</v>
+        <v>4</v>
       </c>
       <c r="AG17">
         <f t="shared" si="2"/>
@@ -17560,7 +17556,7 @@
       </c>
       <c r="AF18">
         <f t="shared" si="2"/>
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="AG18">
         <f t="shared" si="2"/>
@@ -17701,7 +17697,7 @@
       </c>
       <c r="AF19">
         <f t="shared" si="2"/>
-        <v>3.8000000000000003</v>
+        <v>4</v>
       </c>
       <c r="AG19">
         <f t="shared" si="2"/>
@@ -17709,7 +17705,7 @@
       </c>
       <c r="AH19">
         <f t="shared" si="2"/>
-        <v>4.4000000000000004</v>
+        <v>4.6000000000000005</v>
       </c>
       <c r="AI19">
         <f t="shared" si="2"/>
@@ -17983,7 +17979,7 @@
       </c>
       <c r="AF21">
         <f t="shared" si="2"/>
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="AG21">
         <f t="shared" si="2"/>
@@ -18265,7 +18261,7 @@
       </c>
       <c r="AF23">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AG23">
         <f t="shared" si="2"/>

</xml_diff>